<commit_message>
fix bug thue xe
</commit_message>
<xml_diff>
--- a/52100572_52100852_Source_GK/Output/CustomerList.xlsx
+++ b/52100572_52100852_Source_GK/Output/CustomerList.xlsx
@@ -21,32 +21,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+  <si>
+    <t>Spire.XLS for .NET</t>
+  </si>
+  <si>
+    <t>e-iceblue Inc. 2002-2023 All rights reserverd</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>https://www.e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Contact US</t>
+  </si>
+  <si>
+    <t>mailto:support@e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Buy Now!</t>
+  </si>
   <si>
     <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
   </si>
   <si>
-    <t>Buy Now!</t>
-  </si>
-  <si>
-    <t>mailto:support@e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Contact US</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Home page</t>
-  </si>
-  <si>
-    <t>e-iceblue Inc. 2002-2023 All rights reserverd</t>
-  </si>
-  <si>
-    <t>Spire.XLS for .NET</t>
-  </si>
-  <si>
     <t>Mã khách hàng</t>
   </si>
   <si>
@@ -98,31 +98,46 @@
     <t>789 Ðu?ng LMN, Qu?n 3, TP.HCM</t>
   </si>
   <si>
-    <t>sádd</t>
-  </si>
-  <si>
-    <t>adsasd</t>
-  </si>
-  <si>
-    <t>adsdsdsadsad</t>
-  </si>
-  <si>
-    <t>adsadas</t>
-  </si>
-  <si>
-    <t>kúhadasd</t>
-  </si>
-  <si>
-    <t>dsadsad</t>
-  </si>
-  <si>
-    <t>ádds</t>
-  </si>
-  <si>
-    <t>dấd</t>
-  </si>
-  <si>
-    <t>a@gmail.com</t>
+    <t>Phú</t>
+  </si>
+  <si>
+    <t>hehe</t>
+  </si>
+  <si>
+    <t>phu@edu.vn</t>
+  </si>
+  <si>
+    <t>Tây Ninh</t>
+  </si>
+  <si>
+    <t>Phú nè</t>
+  </si>
+  <si>
+    <t>mail@mail.com</t>
+  </si>
+  <si>
+    <t>plplpl@mail.vn</t>
+  </si>
+  <si>
+    <t>Nhà</t>
+  </si>
+  <si>
+    <t>mail@gmail.com</t>
+  </si>
+  <si>
+    <t>m@m.com</t>
+  </si>
+  <si>
+    <t>tn</t>
+  </si>
+  <si>
+    <t>Hiếu gà</t>
+  </si>
+  <si>
+    <t>hieuga2003@gmail.com</t>
+  </si>
+  <si>
+    <t>Lã Xuân Oai</t>
   </si>
 </sst>
 </file>
@@ -182,7 +197,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -206,6 +221,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -257,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="62">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="76">
       <alignment/>
       <protection/>
     </xf>
@@ -269,7 +298,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="62"/>
+    <cellStyle name="Hyperlink" xfId="76"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -614,7 +643,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="H13" sqref="A1:XFD1048576"/>
@@ -697,8 +726,8 @@
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>26</v>
+      <c r="C5">
+        <v>1234567890</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -715,7 +744,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -726,10 +755,70 @@
     </row>
     <row r="7" spans="1:5" ht="15">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -749,42 +838,42 @@
   <sheetData>
     <row r="1" ht="15">
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" ht="15">
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="15">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="15">
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" ht="15">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" ht="15">
       <c r="B8" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" ht="15">
       <c r="B10" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" ht="15">
       <c r="B11" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add ThoiGianTraDK, DiemDen, phoneNumber, email unique
</commit_message>
<xml_diff>
--- a/52100572_52100852_Source_GK/Output/CustomerList.xlsx
+++ b/52100572_52100852_Source_GK/Output/CustomerList.xlsx
@@ -23,30 +23,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
+    <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
+  </si>
+  <si>
+    <t>Buy Now!</t>
+  </si>
+  <si>
+    <t>mailto:support@e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Contact US</t>
+  </si>
+  <si>
+    <t>https://www.e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>e-iceblue Inc. 2002-2023 All rights reserverd</t>
+  </si>
+  <si>
     <t>Spire.XLS for .NET</t>
   </si>
   <si>
-    <t>e-iceblue Inc. 2002-2023 All rights reserverd</t>
-  </si>
-  <si>
-    <t>Home page</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Contact US</t>
-  </si>
-  <si>
-    <t>mailto:support@e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Buy Now!</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
-  </si>
-  <si>
     <t>Mã khách hàng</t>
   </si>
   <si>
@@ -71,7 +71,7 @@
     <t>nguyenvana@example.com</t>
   </si>
   <si>
-    <t>123 Ðu?ng ABC, Qu?n 1, TP.HCM</t>
+    <t>123 Đường ABC, Quận 1, TP.HCM</t>
   </si>
   <si>
     <t>Trần Thị B</t>
@@ -83,7 +83,7 @@
     <t>tranthib@example.com</t>
   </si>
   <si>
-    <t>456 Ðu?ng XYZ, Qu?n 2, TP.HCM</t>
+    <t>456 Đường XYZ, Quận 2, TP.HCM</t>
   </si>
   <si>
     <t>Lê Văn C</t>
@@ -95,7 +95,7 @@
     <t>levanc@example.com</t>
   </si>
   <si>
-    <t>789 Ðu?ng LMN, Qu?n 3, TP.HCM</t>
+    <t>789 Đường LMN, Quận 3, TP.HCM</t>
   </si>
   <si>
     <t>Phú</t>
@@ -197,7 +197,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -221,6 +221,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -286,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="76">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="90">
       <alignment/>
       <protection/>
     </xf>
@@ -298,7 +312,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="76"/>
+    <cellStyle name="Hyperlink" xfId="90"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -838,42 +852,42 @@
   <sheetData>
     <row r="1" ht="15">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" ht="15">
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" ht="15">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" ht="15">
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" ht="15">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" ht="15">
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" ht="15">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" ht="15">
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>